<commit_message>
feat(rapid): team-based rapid round (target=200), winner overlay, admin rapid team selection; P1/P2 % dropdowns incl. 0; wrong sound cue; reset rapid clears awarded points; layout + alignment fixes
</commit_message>
<xml_diff>
--- a/QuestionsAnswers.xlsx
+++ b/QuestionsAnswers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\FamilyFeud\familyfeud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49222E72-643A-4F65-A042-40C8CFD9577A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7715539A-45AA-44A3-AEA1-574532ECD0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="153">
   <si>
     <t>Round</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>പേന / ഉപകരണങ്ങൾ ചെക്ക് ചെയ്യുക</t>
+  </si>
+  <si>
+    <t>ഉറങ്ങാൻ വൈകുന്നത്</t>
   </si>
 </sst>
 </file>
@@ -831,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,7 +1133,9 @@
       <c r="P5" s="1">
         <v>6</v>
       </c>
-      <c r="Q5" s="1"/>
+      <c r="Q5" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="R5" s="1">
         <v>4</v>
       </c>

</xml_diff>